<commit_message>
feat: add lastest data
</commit_message>
<xml_diff>
--- a/out/2023-02-04_cb_list.xlsx
+++ b/out/2023-02-04_cb_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="32700" windowHeight="14960" activeTab="1"/>
+    <workbookView windowHeight="15560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7466" uniqueCount="3910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7467" uniqueCount="3911">
   <si>
     <t>id</t>
   </si>
@@ -11773,6 +11773,9 @@
   </si>
   <si>
     <t>33天</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -11781,11 +11784,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11818,21 +11821,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -11840,10 +11828,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11864,9 +11852,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11879,7 +11875,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11887,14 +11890,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11916,7 +11911,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11931,22 +11934,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11961,7 +11957,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11973,61 +12095,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12039,97 +12113,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12142,6 +12126,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -12179,30 +12175,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -12214,32 +12186,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -12262,24 +12208,68 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -12288,127 +12278,133 @@
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -12769,7 +12765,7 @@
   <dimension ref="A1:AH485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -62589,8 +62585,8 @@
   <sheetPr/>
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="$A8:$XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -63641,10 +63637,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AH11"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="M17" sqref="M17:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -64788,6 +64784,11 @@
       </c>
       <c r="AH11" t="s">
         <v>3398</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8">
+      <c r="H17" t="s">
+        <v>3910</v>
       </c>
     </row>
   </sheetData>
@@ -64801,8 +64802,8 @@
   <sheetPr/>
   <dimension ref="B1:AH1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>